<commit_message>
a little bit flavor
</commit_message>
<xml_diff>
--- a/2/data/loaitruong.xlsx
+++ b/2/data/loaitruong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buivu\Downloads\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519DDB9A-B433-4398-961A-0A05778D3DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61940173-973F-49C3-860B-C98FE623CFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC254833-A69F-46A0-9AA6-07E9AD9B4058}"/>
   </bookViews>
@@ -86,7 +86,7 @@
     <t>Trường chuyên</t>
   </si>
   <si>
-    <t>CHUYE</t>
+    <t>CHUYEN</t>
   </si>
 </sst>
 </file>
@@ -159,14 +159,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +484,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,10 +556,10 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>